<commit_message>
new script to clean template data
</commit_message>
<xml_diff>
--- a/data/digitized_data/dwc_HJ-occurrences_22-11-04.xlsx
+++ b/data/digitized_data/dwc_HJ-occurrences_22-11-04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF4A771-0922-D249-921F-24CD70047AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23863C0E-B59B-4A45-AAEF-FB2120342BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1120" windowWidth="27640" windowHeight="16940" xr2:uid="{C97F215F-9E74-C942-B860-D925B3540C20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{C97F215F-9E74-C942-B860-D925B3540C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1427,7 +1427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1435,7 +1435,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,29 +1752,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A439EF-E6B0-434A-9D0B-4BA1DEE7AC14}">
   <dimension ref="A1:BB93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="AZ21" sqref="AZ21"/>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="10" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="11" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="11" width="6.33203125" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="17" width="9" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="7" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="17" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" customWidth="1"/>
     <col min="23" max="23" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
+    <col min="24" max="24" width="6" customWidth="1"/>
     <col min="25" max="25" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="18.83203125" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
@@ -1787,9 +1787,12 @@
     <col min="36" max="36" width="6.5" customWidth="1"/>
     <col min="37" max="37" width="6.83203125" customWidth="1"/>
     <col min="38" max="38" width="7" customWidth="1"/>
+    <col min="39" max="39" width="10" customWidth="1"/>
     <col min="41" max="41" width="12.1640625" customWidth="1"/>
     <col min="42" max="42" width="12.83203125" customWidth="1"/>
+    <col min="47" max="47" width="16.83203125" customWidth="1"/>
     <col min="48" max="48" width="20.6640625" customWidth="1"/>
+    <col min="51" max="51" width="12.1640625" customWidth="1"/>
     <col min="53" max="53" width="20.6640625" customWidth="1"/>
     <col min="54" max="54" width="49.83203125" customWidth="1"/>
   </cols>
@@ -1954,7 +1957,7 @@
       <c r="BA1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2102,7 +2105,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4">
         <v>27</v>
@@ -2163,7 +2166,7 @@
         <v>70</v>
       </c>
       <c r="B5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4">
         <v>27</v>
@@ -2228,7 +2231,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4">
         <v>27</v>
@@ -2296,7 +2299,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4">
         <v>27</v>
@@ -2367,7 +2370,7 @@
         <v>92</v>
       </c>
       <c r="B8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4">
         <v>27</v>
@@ -2438,7 +2441,7 @@
         <v>93</v>
       </c>
       <c r="B9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>27</v>
@@ -2474,7 +2477,7 @@
         <v>94</v>
       </c>
       <c r="B10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4">
         <v>27</v>
@@ -2512,7 +2515,7 @@
         <v>95</v>
       </c>
       <c r="B11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>27</v>

</xml_diff>